<commit_message>
oh, will update commit message later
</commit_message>
<xml_diff>
--- a/eSMED_settings.xlsx
+++ b/eSMED_settings.xlsx
@@ -5,212 +5,253 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
-  <si>
-    <t>SETINGS</t>
-  </si>
-  <si>
-    <t>SJM</t>
-  </si>
-  <si>
-    <t>JELCZ</t>
-  </si>
-  <si>
-    <t>TRANSLATIONS</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Portuguese</t>
-  </si>
-  <si>
-    <t>Polish</t>
-  </si>
-  <si>
-    <t>Program Window title (CAPS)</t>
-  </si>
-  <si>
-    <t>FAURECIA - CRONÓMETRO DE TROCA DE MOLDES</t>
-  </si>
-  <si>
-    <t>FAURECIA e-SMED</t>
-  </si>
-  <si>
-    <t>Line (CAPS)</t>
-  </si>
-  <si>
-    <t>LINHA</t>
-  </si>
-  <si>
-    <t>LINIA</t>
-  </si>
-  <si>
-    <t>Program title (CAPS)</t>
-  </si>
-  <si>
-    <t>CRONÓMETRO DE MUDANÇA DE MOLDES</t>
-  </si>
-  <si>
-    <t>eSmed – JELCZ
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+  <si>
+    <t xml:space="preserve">SETINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JELCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSLATIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portuguese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Window title (CAPS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAURECIA - CRONÓMETRO DE TROCA DE MOLDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAURECIA e-SMED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line (CAPS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program title (CAPS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRONÓMETRO DE MUDANÇA DE MOLDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eSmed – JELCZ
 STACJA WYMIANY FORM – LINIA 3</t>
   </si>
   <si>
-    <t>Last times</t>
-  </si>
-  <si>
-    <t>Últimos tempos</t>
-  </si>
-  <si>
-    <t>Ostatni czs</t>
-  </si>
-  <si>
-    <t>Plant name (CAPS)</t>
-  </si>
-  <si>
-    <t>FAA MOLDADOS</t>
-  </si>
-  <si>
-    <t>JELCZ-FOAM</t>
-  </si>
-  <si>
-    <t>Date/Hour</t>
-  </si>
-  <si>
-    <t>Data/Hora</t>
-  </si>
-  <si>
-    <t>Data/Godzina</t>
-  </si>
-  <si>
-    <t>Line number</t>
-  </si>
-  <si>
-    <t>we have 3 lines(#2,#3,#4)</t>
-  </si>
-  <si>
-    <t>Best times</t>
-  </si>
-  <si>
-    <t>Melhores tempos</t>
-  </si>
-  <si>
-    <t>Najlepszy czas przezbrojenia</t>
-  </si>
-  <si>
-    <t>Green to Yellow goal time seconds</t>
-  </si>
-  <si>
-    <t>Can we have this in settings as editable value??</t>
-  </si>
-  <si>
-    <t>Goal time</t>
-  </si>
-  <si>
-    <t>Tempo objectivo</t>
-  </si>
-  <si>
-    <t>Cel-czas przezbrojenia</t>
-  </si>
-  <si>
-    <t>Yellow to red goal time seconds</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>Definições</t>
-  </si>
-  <si>
-    <t>Ustawienia</t>
-  </si>
-  <si>
-    <t>Lowest time acceptable seconds</t>
-  </si>
-  <si>
-    <t>Export data</t>
-  </si>
-  <si>
-    <t>Exportar dados</t>
-  </si>
-  <si>
-    <t>Prześlij dane</t>
-  </si>
-  <si>
-    <t>Highest time acceptable seconds</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Fechar</t>
-  </si>
-  <si>
-    <t>Zamknięcie</t>
-  </si>
-  <si>
-    <t>password to exit program</t>
-  </si>
-  <si>
-    <t>raspberry</t>
-  </si>
-  <si>
-    <t>Insert password:</t>
-  </si>
-  <si>
-    <t>Insira a password:</t>
-  </si>
-  <si>
-    <t>Podaj hasło</t>
-  </si>
-  <si>
-    <t>Wrong password!</t>
-  </si>
-  <si>
-    <t>Password Errada!</t>
-  </si>
-  <si>
-    <t>Hasło nieprawidłowe</t>
-  </si>
-  <si>
-    <t>Program language</t>
-  </si>
-  <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>Change Language</t>
-  </si>
-  <si>
-    <t>Mudar idioma</t>
-  </si>
-  <si>
-    <t>Zmiana Języka</t>
-  </si>
-  <si>
-    <t>Português</t>
-  </si>
-  <si>
-    <t>Portugalski</t>
-  </si>
-  <si>
-    <t>Polaco</t>
-  </si>
-  <si>
-    <t>Polski</t>
+    <t xml:space="preserve">Last times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Últimos tempos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ostatni czas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant name (CAPS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAA MOLDADOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JELCZ-FOAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date/Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Godzina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we have 3 lines(#2,#3,#4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melhores tempos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Najlepszy czas przezbrojenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green to Yellow goal time seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can we have this in settings as editable value??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo objectivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cel-czas przezbrojenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow to red goal time seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definições</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ustawienia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lowest time acceptable seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportar dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prześlij dane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highest time acceptable seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fechar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zamknięcie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password to exit program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raspberry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert password:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insira a password:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podaj hasło</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong password!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password Errada!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasło nieprawidłowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mudar idioma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zmiana Języka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Português</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugalski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polaco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged in:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON-LINE:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zalogowany:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in before starting!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login antes de começar a trabalhar!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaloguj się przed rozpoczęciem pracy!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login necessário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konieczne zalogowanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usuário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kto?</t>
   </si>
 </sst>
 </file>
@@ -218,7 +259,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -291,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -301,6 +342,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,24 +426,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.82589285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.3348214285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.0044642857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4955357142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8258928571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6607142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.82589285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +706,48 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="1"/>
+      <c r="G15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
removed messagebox for expanding label (to not loose focus on lineedit)
</commit_message>
<xml_diff>
--- a/eSMED_settings.xlsx
+++ b/eSMED_settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t xml:space="preserve">SETINGS</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t xml:space="preserve">Kto?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to login before continuing (use your RFID card)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precisa fazer o login antes de continuar (use seu cartão RFID)</t>
   </si>
 </sst>
 </file>
@@ -426,24 +432,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,6 +753,17 @@
       </c>
       <c r="I18" s="0" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>